<commit_message>
adding more experimental climate data
</commit_message>
<xml_diff>
--- a/Experiments/exp_site_info.xlsx
+++ b/Experiments/exp_site_info.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="26621"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="720" yWindow="720" windowWidth="24880" windowHeight="15940" tabRatio="500"/>
+    <workbookView xWindow="720" yWindow="700" windowWidth="24880" windowHeight="16000" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="165" uniqueCount="98">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="174" uniqueCount="107">
   <si>
     <t xml:space="preserve">Source
 </t>
@@ -314,6 +314,33 @@
   </si>
   <si>
     <t>soilmois_freq_hr</t>
+  </si>
+  <si>
+    <t>Sitename</t>
+  </si>
+  <si>
+    <t>price</t>
+  </si>
+  <si>
+    <t>marchin</t>
+  </si>
+  <si>
+    <t>bace</t>
+  </si>
+  <si>
+    <t>clarkduke</t>
+  </si>
+  <si>
+    <t>clarkharvard</t>
+  </si>
+  <si>
+    <t>cleland</t>
+  </si>
+  <si>
+    <t>sherry</t>
+  </si>
+  <si>
+    <t>farnsworth</t>
   </si>
 </sst>
 </file>
@@ -340,12 +367,18 @@
       <name val="Arial"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="2">
@@ -375,7 +408,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
@@ -383,6 +416,12 @@
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -714,7 +753,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AI12"/>
+  <dimension ref="A1:AJ12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="C5" sqref="C5"/>
@@ -722,33 +761,33 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>
-    <col min="1" max="2" width="10.83203125" style="2"/>
-    <col min="3" max="3" width="37.5" style="2" customWidth="1"/>
-    <col min="4" max="4" width="16" style="2" customWidth="1"/>
-    <col min="5" max="5" width="10.83203125" style="2"/>
-    <col min="6" max="6" width="20" style="2" customWidth="1"/>
-    <col min="7" max="8" width="10.83203125" style="2"/>
-    <col min="9" max="9" width="24.33203125" style="2" customWidth="1"/>
-    <col min="10" max="12" width="10.83203125" style="2"/>
-    <col min="13" max="13" width="35" style="2" customWidth="1"/>
-    <col min="14" max="15" width="10.83203125" style="2"/>
-    <col min="16" max="16" width="11.6640625" style="2" customWidth="1"/>
-    <col min="17" max="17" width="16" style="2" customWidth="1"/>
-    <col min="18" max="18" width="13.83203125" style="2" customWidth="1"/>
-    <col min="19" max="19" width="14.83203125" style="2" customWidth="1"/>
-    <col min="20" max="20" width="15.83203125" style="2" customWidth="1"/>
-    <col min="21" max="22" width="10.83203125" style="2"/>
-    <col min="23" max="23" width="15" style="2" customWidth="1"/>
-    <col min="24" max="24" width="15.6640625" style="2" customWidth="1"/>
-    <col min="25" max="25" width="16.6640625" style="2" customWidth="1"/>
-    <col min="26" max="26" width="20.6640625" style="2" customWidth="1"/>
-    <col min="27" max="27" width="21" style="2" customWidth="1"/>
-    <col min="28" max="28" width="22" style="2" customWidth="1"/>
-    <col min="29" max="33" width="16.5" style="2" customWidth="1"/>
-    <col min="34" max="16384" width="10.83203125" style="2"/>
+    <col min="1" max="3" width="10.83203125" style="2"/>
+    <col min="4" max="4" width="37.5" style="2" customWidth="1"/>
+    <col min="5" max="5" width="16" style="2" customWidth="1"/>
+    <col min="6" max="6" width="10.83203125" style="2"/>
+    <col min="7" max="7" width="20" style="2" customWidth="1"/>
+    <col min="8" max="9" width="10.83203125" style="2"/>
+    <col min="10" max="10" width="24.33203125" style="2" customWidth="1"/>
+    <col min="11" max="13" width="10.83203125" style="2"/>
+    <col min="14" max="14" width="35" style="2" customWidth="1"/>
+    <col min="15" max="16" width="10.83203125" style="2"/>
+    <col min="17" max="17" width="11.6640625" style="2" customWidth="1"/>
+    <col min="18" max="18" width="16" style="2" customWidth="1"/>
+    <col min="19" max="19" width="13.83203125" style="2" customWidth="1"/>
+    <col min="20" max="20" width="14.83203125" style="2" customWidth="1"/>
+    <col min="21" max="21" width="15.83203125" style="2" customWidth="1"/>
+    <col min="22" max="23" width="10.83203125" style="2"/>
+    <col min="24" max="24" width="15" style="2" customWidth="1"/>
+    <col min="25" max="25" width="15.6640625" style="2" customWidth="1"/>
+    <col min="26" max="26" width="16.6640625" style="2" customWidth="1"/>
+    <col min="27" max="27" width="20.6640625" style="2" customWidth="1"/>
+    <col min="28" max="28" width="21" style="2" customWidth="1"/>
+    <col min="29" max="29" width="22" style="2" customWidth="1"/>
+    <col min="30" max="34" width="16.5" style="2" customWidth="1"/>
+    <col min="35" max="16384" width="10.83203125" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:35" ht="17" thickBot="1">
+    <row r="1" spans="1:36" ht="17" thickBot="1">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -756,100 +795,103 @@
         <v>1</v>
       </c>
       <c r="C1" s="1" t="s">
+        <v>98</v>
+      </c>
+      <c r="D1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="E1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="F1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="G1" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="H1" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="I1" s="1" t="s">
         <v>88</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="J1" s="1" t="s">
         <v>89</v>
       </c>
-      <c r="J1" s="1"/>
-      <c r="K1" s="1" t="s">
+      <c r="K1" s="1"/>
+      <c r="L1" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="L1" s="1" t="s">
+      <c r="M1" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="M1" s="1" t="s">
+      <c r="N1" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="N1" s="1" t="s">
+      <c r="O1" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="O1" s="1" t="s">
+      <c r="P1" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="P1" s="1" t="s">
+      <c r="Q1" s="1" t="s">
         <v>87</v>
       </c>
-      <c r="Q1" s="1" t="s">
+      <c r="R1" s="1" t="s">
         <v>90</v>
       </c>
-      <c r="R1" s="1" t="s">
+      <c r="S1" s="1" t="s">
         <v>91</v>
       </c>
-      <c r="S1" s="1" t="s">
+      <c r="T1" s="1" t="s">
         <v>92</v>
       </c>
-      <c r="T1" s="1" t="s">
+      <c r="U1" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="U1" s="1" t="s">
+      <c r="V1" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="V1" s="1" t="s">
+      <c r="W1" s="1" t="s">
         <v>93</v>
       </c>
-      <c r="W1" s="1" t="s">
+      <c r="X1" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="X1" s="1" t="s">
+      <c r="Y1" s="1" t="s">
         <v>94</v>
       </c>
-      <c r="Y1" s="1" t="s">
+      <c r="Z1" s="1" t="s">
         <v>95</v>
       </c>
-      <c r="Z1" s="1" t="s">
+      <c r="AA1" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="AA1" s="1" t="s">
+      <c r="AB1" s="1" t="s">
         <v>96</v>
       </c>
-      <c r="AB1" s="1" t="s">
+      <c r="AC1" s="1" t="s">
         <v>97</v>
       </c>
-      <c r="AC1" s="1" t="s">
+      <c r="AD1" s="1" t="s">
         <v>80</v>
       </c>
-      <c r="AD1" s="1" t="s">
+      <c r="AE1" s="1" t="s">
         <v>81</v>
       </c>
-      <c r="AE1" s="1" t="s">
+      <c r="AF1" s="1" t="s">
         <v>82</v>
       </c>
-      <c r="AF1" s="1" t="s">
+      <c r="AG1" s="1" t="s">
         <v>83</v>
       </c>
-      <c r="AG1" s="1" t="s">
+      <c r="AH1" s="1" t="s">
         <v>84</v>
       </c>
-      <c r="AH1" s="1"/>
       <c r="AI1" s="1"/>
+      <c r="AJ1" s="1"/>
     </row>
-    <row r="2" spans="1:35" ht="17" thickBot="1">
+    <row r="2" spans="1:36" ht="17" thickBot="1">
       <c r="A2" s="1" t="s">
         <v>16</v>
       </c>
@@ -857,185 +899,191 @@
         <v>17</v>
       </c>
       <c r="C2" s="1" t="s">
+        <v>99</v>
+      </c>
+      <c r="D2" s="1" t="s">
         <v>86</v>
       </c>
-      <c r="D2" s="1" t="s">
+      <c r="E2" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="E2" s="3">
+      <c r="F2" s="3">
         <v>1998</v>
       </c>
-      <c r="F2" s="1" t="s">
+      <c r="G2" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="G2" s="3">
+      <c r="H2" s="3">
         <v>79</v>
       </c>
-      <c r="H2" s="3">
+      <c r="I2" s="3">
         <v>1261</v>
       </c>
-      <c r="I2" s="1" t="s">
+      <c r="J2" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="J2" s="1"/>
-      <c r="K2" s="1" t="s">
+      <c r="K2" s="1"/>
+      <c r="L2" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="L2" s="3">
+      <c r="M2" s="3">
         <v>10</v>
       </c>
-      <c r="M2" s="1" t="s">
+      <c r="N2" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="N2" s="3">
+      <c r="O2" s="3">
         <v>38.883000000000003</v>
       </c>
-      <c r="O2" s="3">
+      <c r="P2" s="3">
         <v>-107.033</v>
       </c>
-      <c r="P2" s="3">
+      <c r="Q2" s="3">
         <v>2920</v>
       </c>
-      <c r="Q2" s="3">
+      <c r="R2" s="3">
         <v>1991</v>
       </c>
-      <c r="R2" s="3">
+      <c r="S2" s="3">
         <v>1994</v>
       </c>
-      <c r="S2" s="3">
+      <c r="T2" s="3">
         <v>1990</v>
       </c>
-      <c r="T2" s="3">
+      <c r="U2" s="3">
         <v>7</v>
       </c>
-      <c r="U2" s="1"/>
-      <c r="V2" s="1" t="s">
+      <c r="V2" s="1"/>
+      <c r="W2" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="W2" s="1" t="s">
+      <c r="X2" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="X2" s="1" t="s">
+      <c r="Y2" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="Y2" s="1" t="s">
+      <c r="Z2" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="Z2" s="1" t="s">
+      <c r="AA2" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="AA2" s="3">
+      <c r="AB2" s="3">
         <v>2</v>
       </c>
-      <c r="AB2" s="1" t="s">
+      <c r="AC2" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="AC2" s="1">
+      <c r="AD2" s="1">
         <v>5</v>
       </c>
-      <c r="AD2" s="1">
+      <c r="AE2" s="1">
         <v>12</v>
       </c>
-      <c r="AE2" s="1">
+      <c r="AF2" s="1">
         <v>25</v>
       </c>
-      <c r="AF2" s="1"/>
       <c r="AG2" s="1"/>
       <c r="AH2" s="1"/>
       <c r="AI2" s="1"/>
+      <c r="AJ2" s="1"/>
     </row>
-    <row r="3" spans="1:35" ht="17" thickBot="1">
-      <c r="A3" s="4" t="s">
+    <row r="3" spans="1:36" s="8" customFormat="1" ht="17" thickBot="1">
+      <c r="A3" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="B3" s="1" t="s">
+      <c r="B3" s="6" t="s">
         <v>28</v>
       </c>
-      <c r="C3" s="1" t="s">
+      <c r="C3" s="6" t="s">
+        <v>100</v>
+      </c>
+      <c r="D3" s="6" t="s">
         <v>29</v>
       </c>
-      <c r="D3" s="1" t="s">
+      <c r="E3" s="6" t="s">
         <v>30</v>
       </c>
-      <c r="E3" s="3">
+      <c r="F3" s="7">
         <v>2015</v>
       </c>
-      <c r="F3" s="1" t="s">
+      <c r="G3" s="6" t="s">
         <v>31</v>
       </c>
-      <c r="G3" s="3">
+      <c r="H3" s="7">
         <v>21</v>
       </c>
-      <c r="H3" s="3">
+      <c r="I3" s="7">
         <v>3138</v>
       </c>
-      <c r="I3" s="1" t="s">
+      <c r="J3" s="6" t="s">
         <v>21</v>
       </c>
-      <c r="J3" s="1"/>
-      <c r="K3" s="1"/>
-      <c r="L3" s="3">
+      <c r="K3" s="6"/>
+      <c r="L3" s="6"/>
+      <c r="M3" s="7">
         <v>11</v>
       </c>
-      <c r="M3" s="1" t="s">
+      <c r="N3" s="6" t="s">
         <v>32</v>
       </c>
-      <c r="N3" s="3">
+      <c r="O3" s="7">
         <v>36</v>
       </c>
-      <c r="O3" s="3">
+      <c r="P3" s="7">
         <v>-79.099999999999994</v>
       </c>
-      <c r="P3" s="3">
+      <c r="Q3" s="7">
         <v>130</v>
       </c>
-      <c r="Q3" s="3">
+      <c r="R3" s="7">
         <v>2010</v>
       </c>
-      <c r="R3" s="3">
+      <c r="S3" s="7">
         <v>2012</v>
       </c>
-      <c r="S3" s="3">
+      <c r="T3" s="7">
         <v>2010</v>
       </c>
-      <c r="T3" s="3">
+      <c r="U3" s="7">
         <v>7</v>
       </c>
-      <c r="U3" s="1"/>
-      <c r="V3" s="1" t="s">
+      <c r="V3" s="6"/>
+      <c r="W3" s="6" t="s">
         <v>33</v>
       </c>
-      <c r="W3" s="1" t="s">
+      <c r="X3" s="6" t="s">
         <v>34</v>
       </c>
-      <c r="X3" s="1" t="s">
+      <c r="Y3" s="6" t="s">
         <v>26</v>
       </c>
-      <c r="Y3" s="1" t="s">
+      <c r="Z3" s="6" t="s">
         <v>35</v>
       </c>
-      <c r="Z3" s="1">
+      <c r="AA3" s="6">
         <v>1</v>
       </c>
-      <c r="AA3" s="1">
+      <c r="AB3" s="6">
         <v>1</v>
       </c>
-      <c r="AB3" s="1">
+      <c r="AC3" s="6">
         <v>1</v>
       </c>
-      <c r="AC3" s="1">
+      <c r="AD3" s="6">
         <v>2</v>
       </c>
-      <c r="AD3" s="1">
+      <c r="AE3" s="6">
         <v>6</v>
       </c>
-      <c r="AE3" s="1"/>
-      <c r="AF3" s="1"/>
-      <c r="AG3" s="1"/>
-      <c r="AH3" s="1"/>
-      <c r="AI3" s="1"/>
+      <c r="AF3" s="6"/>
+      <c r="AG3" s="6"/>
+      <c r="AH3" s="6"/>
+      <c r="AI3" s="6"/>
+      <c r="AJ3" s="6"/>
     </row>
-    <row r="4" spans="1:35" ht="17" thickBot="1">
+    <row r="4" spans="1:36" ht="17" thickBot="1">
       <c r="A4" s="4" t="s">
         <v>16</v>
       </c>
@@ -1043,13 +1091,13 @@
         <v>36</v>
       </c>
       <c r="C4" s="1" t="s">
+        <v>101</v>
+      </c>
+      <c r="D4" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="D4" s="1" t="s">
+      <c r="E4" s="1" t="s">
         <v>38</v>
-      </c>
-      <c r="E4" s="1" t="s">
-        <v>27</v>
       </c>
       <c r="F4" s="1" t="s">
         <v>27</v>
@@ -1061,70 +1109,73 @@
         <v>27</v>
       </c>
       <c r="I4" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="J4" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="J4" s="1"/>
-      <c r="K4" s="1" t="s">
+      <c r="K4" s="1"/>
+      <c r="L4" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="L4" s="3">
+      <c r="M4" s="3">
         <v>18</v>
       </c>
-      <c r="M4" s="1" t="s">
+      <c r="N4" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="N4" s="3">
+      <c r="O4" s="3">
         <v>42.383987599999998</v>
       </c>
-      <c r="O4" s="3">
+      <c r="P4" s="3">
         <v>-71.212284600000004</v>
       </c>
-      <c r="P4" s="3">
+      <c r="Q4" s="3">
         <v>18</v>
       </c>
-      <c r="Q4" s="3">
+      <c r="R4" s="3">
         <v>2010</v>
       </c>
-      <c r="R4" s="3">
+      <c r="S4" s="3">
         <v>2011</v>
       </c>
-      <c r="S4" s="3">
+      <c r="T4" s="3">
         <v>2009</v>
       </c>
-      <c r="T4" s="1"/>
       <c r="U4" s="1"/>
-      <c r="V4" s="1" t="s">
+      <c r="V4" s="1"/>
+      <c r="W4" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="W4" s="1" t="s">
+      <c r="X4" s="1" t="s">
         <v>34</v>
-      </c>
-      <c r="X4" s="1" t="s">
-        <v>35</v>
       </c>
       <c r="Y4" s="1" t="s">
         <v>35</v>
       </c>
       <c r="Z4" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="AA4" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="AA4" s="3">
+      <c r="AB4" s="3">
         <v>24</v>
       </c>
-      <c r="AB4" s="3">
+      <c r="AC4" s="3">
         <v>240</v>
       </c>
-      <c r="AC4" s="3">
+      <c r="AD4" s="3">
         <v>30</v>
       </c>
-      <c r="AD4" s="1"/>
       <c r="AE4" s="1"/>
       <c r="AF4" s="1"/>
       <c r="AG4" s="1"/>
       <c r="AH4" s="1"/>
       <c r="AI4" s="1"/>
+      <c r="AJ4" s="1"/>
     </row>
-    <row r="5" spans="1:35" ht="17" thickBot="1">
+    <row r="5" spans="1:36" ht="17" thickBot="1">
       <c r="A5" s="1" t="s">
         <v>16</v>
       </c>
@@ -1132,70 +1183,70 @@
         <v>40</v>
       </c>
       <c r="C5" s="1" t="s">
+        <v>102</v>
+      </c>
+      <c r="D5" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="D5" s="1" t="s">
+      <c r="E5" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="E5" s="3">
+      <c r="F5" s="3">
         <v>2014</v>
       </c>
-      <c r="F5" s="1" t="s">
+      <c r="G5" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="G5" s="3">
+      <c r="H5" s="3">
         <v>28</v>
       </c>
-      <c r="H5" s="3">
+      <c r="I5" s="3">
         <v>1344</v>
       </c>
-      <c r="I5" s="1" t="s">
+      <c r="J5" s="1" t="s">
         <v>43</v>
       </c>
-      <c r="J5" s="1"/>
       <c r="K5" s="1"/>
-      <c r="L5" s="3">
+      <c r="L5" s="1"/>
+      <c r="M5" s="3">
         <v>15</v>
       </c>
-      <c r="M5" s="1" t="s">
+      <c r="N5" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="N5" s="3">
+      <c r="O5" s="3">
         <v>36</v>
       </c>
-      <c r="O5" s="3">
+      <c r="P5" s="3">
         <v>-79.099999999999994</v>
       </c>
-      <c r="P5" s="3">
+      <c r="Q5" s="3">
         <v>130</v>
       </c>
-      <c r="Q5" s="3">
+      <c r="R5" s="3">
         <v>2009</v>
       </c>
-      <c r="R5" s="3">
+      <c r="S5" s="3">
         <v>2012</v>
       </c>
-      <c r="S5" s="3">
+      <c r="T5" s="3">
         <v>2009</v>
       </c>
-      <c r="T5" s="3">
+      <c r="U5" s="3">
         <v>7</v>
       </c>
-      <c r="U5" s="1"/>
-      <c r="V5" s="1" t="s">
+      <c r="V5" s="1"/>
+      <c r="W5" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="W5" s="1" t="s">
+      <c r="X5" s="1" t="s">
         <v>85</v>
       </c>
-      <c r="X5" s="1" t="s">
+      <c r="Y5" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="Y5" s="1" t="s">
+      <c r="Z5" s="1" t="s">
         <v>35</v>
-      </c>
-      <c r="Z5" s="1">
-        <v>1</v>
       </c>
       <c r="AA5" s="1">
         <v>1</v>
@@ -1203,17 +1254,20 @@
       <c r="AB5" s="1">
         <v>1</v>
       </c>
-      <c r="AC5" s="3">
+      <c r="AC5" s="1">
+        <v>1</v>
+      </c>
+      <c r="AD5" s="3">
         <v>10</v>
       </c>
-      <c r="AD5" s="1"/>
       <c r="AE5" s="1"/>
       <c r="AF5" s="1"/>
       <c r="AG5" s="1"/>
       <c r="AH5" s="1"/>
       <c r="AI5" s="1"/>
+      <c r="AJ5" s="1"/>
     </row>
-    <row r="6" spans="1:35" ht="17" thickBot="1">
+    <row r="6" spans="1:36" ht="17" thickBot="1">
       <c r="A6" s="1" t="s">
         <v>16</v>
       </c>
@@ -1221,70 +1275,70 @@
         <v>45</v>
       </c>
       <c r="C6" s="1" t="s">
+        <v>103</v>
+      </c>
+      <c r="D6" s="1" t="s">
         <v>46</v>
       </c>
-      <c r="D6" s="1" t="s">
+      <c r="E6" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="E6" s="3">
+      <c r="F6" s="3">
         <v>2014</v>
       </c>
-      <c r="F6" s="1" t="s">
+      <c r="G6" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="G6" s="3">
+      <c r="H6" s="3">
         <v>28</v>
       </c>
-      <c r="H6" s="3">
+      <c r="I6" s="3">
         <v>1344</v>
       </c>
-      <c r="I6" s="1" t="s">
+      <c r="J6" s="1" t="s">
         <v>43</v>
       </c>
-      <c r="J6" s="1"/>
       <c r="K6" s="1"/>
-      <c r="L6" s="3">
+      <c r="L6" s="1"/>
+      <c r="M6" s="3">
         <v>15</v>
       </c>
-      <c r="M6" s="1" t="s">
+      <c r="N6" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="N6" s="3">
+      <c r="O6" s="3">
         <v>42.5</v>
       </c>
-      <c r="O6" s="3">
+      <c r="P6" s="3">
         <v>-72.2</v>
       </c>
-      <c r="P6" s="3">
+      <c r="Q6" s="3">
         <v>340</v>
       </c>
-      <c r="Q6" s="3">
+      <c r="R6" s="3">
         <v>2009</v>
       </c>
-      <c r="R6" s="3">
+      <c r="S6" s="3">
         <v>2012</v>
       </c>
-      <c r="S6" s="3">
+      <c r="T6" s="3">
         <v>2009</v>
       </c>
-      <c r="T6" s="3">
+      <c r="U6" s="3">
         <v>7</v>
       </c>
-      <c r="U6" s="1"/>
-      <c r="V6" s="1" t="s">
+      <c r="V6" s="1"/>
+      <c r="W6" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="W6" s="1" t="s">
+      <c r="X6" s="1" t="s">
         <v>85</v>
       </c>
-      <c r="X6" s="1" t="s">
+      <c r="Y6" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="Y6" s="1" t="s">
+      <c r="Z6" s="1" t="s">
         <v>35</v>
-      </c>
-      <c r="Z6" s="1">
-        <v>1</v>
       </c>
       <c r="AA6" s="1">
         <v>1</v>
@@ -1292,17 +1346,20 @@
       <c r="AB6" s="1">
         <v>1</v>
       </c>
-      <c r="AC6" s="3">
+      <c r="AC6" s="1">
+        <v>1</v>
+      </c>
+      <c r="AD6" s="3">
         <v>10</v>
       </c>
-      <c r="AD6" s="1"/>
       <c r="AE6" s="1"/>
       <c r="AF6" s="1"/>
       <c r="AG6" s="1"/>
       <c r="AH6" s="1"/>
       <c r="AI6" s="1"/>
+      <c r="AJ6" s="1"/>
     </row>
-    <row r="7" spans="1:35" ht="17" thickBot="1">
+    <row r="7" spans="1:36" ht="17" thickBot="1">
       <c r="A7" s="1" t="s">
         <v>47</v>
       </c>
@@ -1310,90 +1367,93 @@
         <v>48</v>
       </c>
       <c r="C7" s="1" t="s">
+        <v>104</v>
+      </c>
+      <c r="D7" s="1" t="s">
         <v>49</v>
       </c>
-      <c r="D7" s="1" t="s">
+      <c r="E7" s="1" t="s">
         <v>50</v>
       </c>
-      <c r="E7" s="3">
+      <c r="F7" s="3">
         <v>2006</v>
       </c>
-      <c r="F7" s="1" t="s">
+      <c r="G7" s="1" t="s">
         <v>51</v>
       </c>
-      <c r="G7" s="3">
+      <c r="H7" s="3">
         <v>103</v>
       </c>
-      <c r="H7" s="3">
+      <c r="I7" s="3">
         <v>13740</v>
       </c>
-      <c r="I7" s="1" t="s">
+      <c r="J7" s="1" t="s">
         <v>52</v>
       </c>
-      <c r="J7" s="1"/>
-      <c r="K7" s="1" t="s">
+      <c r="K7" s="1"/>
+      <c r="L7" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="L7" s="3">
+      <c r="M7" s="3">
         <v>9</v>
       </c>
-      <c r="M7" s="1" t="s">
+      <c r="N7" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="N7" s="3">
+      <c r="O7" s="3">
         <v>37.24</v>
       </c>
-      <c r="O7" s="3">
+      <c r="P7" s="3">
         <v>-122.14</v>
       </c>
-      <c r="P7" s="3">
+      <c r="Q7" s="3">
         <v>120</v>
       </c>
-      <c r="Q7" s="3">
+      <c r="R7" s="3">
         <v>2000</v>
       </c>
-      <c r="R7" s="3">
+      <c r="S7" s="3">
         <v>2002</v>
       </c>
-      <c r="S7" s="3">
+      <c r="T7" s="3">
         <v>1998</v>
       </c>
-      <c r="T7" s="3">
+      <c r="U7" s="3">
         <v>3</v>
       </c>
-      <c r="U7" s="1"/>
-      <c r="V7" s="1" t="s">
+      <c r="V7" s="1"/>
+      <c r="W7" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="W7" s="1" t="s">
+      <c r="X7" s="1" t="s">
         <v>53</v>
       </c>
-      <c r="X7" s="1" t="s">
+      <c r="Y7" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="Y7" s="1" t="s">
+      <c r="Z7" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="Z7" s="1" t="s">
+      <c r="AA7" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="AA7" s="3">
+      <c r="AB7" s="3">
         <v>744</v>
       </c>
-      <c r="AB7" s="3">
+      <c r="AC7" s="3">
         <v>8760</v>
       </c>
-      <c r="AC7" s="3">
+      <c r="AD7" s="3">
         <v>15</v>
       </c>
-      <c r="AD7" s="1"/>
       <c r="AE7" s="1"/>
       <c r="AF7" s="1"/>
       <c r="AG7" s="1"/>
       <c r="AH7" s="1"/>
       <c r="AI7" s="1"/>
+      <c r="AJ7" s="1"/>
     </row>
-    <row r="8" spans="1:35" ht="17" thickBot="1">
+    <row r="8" spans="1:36" ht="17" thickBot="1">
       <c r="A8" s="1" t="s">
         <v>47</v>
       </c>
@@ -1401,72 +1461,72 @@
         <v>54</v>
       </c>
       <c r="C8" s="1" t="s">
+        <v>105</v>
+      </c>
+      <c r="D8" s="1" t="s">
         <v>55</v>
       </c>
-      <c r="D8" s="1" t="s">
+      <c r="E8" s="1" t="s">
         <v>56</v>
       </c>
-      <c r="E8" s="3">
+      <c r="F8" s="3">
         <v>2007</v>
       </c>
-      <c r="F8" s="1" t="s">
+      <c r="G8" s="1" t="s">
         <v>51</v>
       </c>
-      <c r="G8" s="3">
+      <c r="H8" s="3">
         <v>104</v>
       </c>
-      <c r="H8" s="3">
+      <c r="I8" s="3">
         <v>198</v>
       </c>
-      <c r="I8" s="1" t="s">
+      <c r="J8" s="1" t="s">
         <v>52</v>
       </c>
-      <c r="J8" s="1"/>
-      <c r="K8" s="1" t="s">
+      <c r="K8" s="1"/>
+      <c r="L8" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="L8" s="3">
+      <c r="M8" s="3">
         <v>12</v>
       </c>
-      <c r="M8" s="1" t="s">
+      <c r="N8" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="N8" s="3">
+      <c r="O8" s="3">
         <v>34.58</v>
       </c>
-      <c r="O8" s="3">
+      <c r="P8" s="3">
         <v>-97.31</v>
       </c>
-      <c r="P8" s="3">
+      <c r="Q8" s="3">
         <v>339</v>
       </c>
-      <c r="Q8" s="3">
+      <c r="R8" s="3">
         <v>2003</v>
       </c>
-      <c r="R8" s="3">
+      <c r="S8" s="3">
         <v>2004</v>
       </c>
-      <c r="S8" s="3">
+      <c r="T8" s="3">
         <v>2003</v>
       </c>
-      <c r="T8" s="3">
+      <c r="U8" s="3">
         <v>14</v>
       </c>
-      <c r="U8" s="1"/>
-      <c r="V8" s="1" t="s">
+      <c r="V8" s="1"/>
+      <c r="W8" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="W8" s="1" t="s">
+      <c r="X8" s="1" t="s">
         <v>57</v>
       </c>
-      <c r="X8" s="1" t="s">
+      <c r="Y8" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="Y8" s="1" t="s">
+      <c r="Z8" s="1" t="s">
         <v>26</v>
-      </c>
-      <c r="Z8" s="3">
-        <v>1</v>
       </c>
       <c r="AA8" s="3">
         <v>1</v>
@@ -1474,195 +1534,197 @@
       <c r="AB8" s="3">
         <v>1</v>
       </c>
-      <c r="AC8" s="1">
+      <c r="AC8" s="3">
+        <v>1</v>
+      </c>
+      <c r="AD8" s="1">
         <v>7.5</v>
       </c>
-      <c r="AD8" s="1">
+      <c r="AE8" s="1">
         <v>22.5</v>
       </c>
-      <c r="AE8" s="1">
+      <c r="AF8" s="1">
         <v>45</v>
       </c>
-      <c r="AF8" s="1">
+      <c r="AG8" s="1">
         <v>75</v>
       </c>
-      <c r="AG8" s="1">
+      <c r="AH8" s="1">
         <v>105</v>
       </c>
-      <c r="AH8" s="1"/>
       <c r="AI8" s="1"/>
+      <c r="AJ8" s="1"/>
     </row>
-    <row r="9" spans="1:35" ht="17" thickBot="1">
+    <row r="9" spans="1:36" ht="17" thickBot="1">
       <c r="A9" s="1" t="s">
         <v>47</v>
       </c>
       <c r="B9" s="1" t="s">
         <v>58</v>
       </c>
-      <c r="C9" s="1" t="s">
+      <c r="C9" s="1"/>
+      <c r="D9" s="1" t="s">
         <v>59</v>
       </c>
-      <c r="D9" s="1" t="s">
+      <c r="E9" s="1" t="s">
         <v>60</v>
       </c>
-      <c r="E9" s="3">
+      <c r="F9" s="3">
         <v>2008</v>
       </c>
-      <c r="F9" s="1" t="s">
+      <c r="G9" s="1" t="s">
         <v>61</v>
       </c>
-      <c r="G9" s="3">
+      <c r="H9" s="3">
         <v>40</v>
       </c>
-      <c r="H9" s="3">
+      <c r="I9" s="3">
         <v>249</v>
       </c>
-      <c r="I9" s="1" t="s">
+      <c r="J9" s="1" t="s">
         <v>62</v>
       </c>
-      <c r="J9" s="1"/>
-      <c r="K9" s="1" t="s">
+      <c r="K9" s="1"/>
+      <c r="L9" s="1" t="s">
         <v>63</v>
       </c>
-      <c r="L9" s="3">
+      <c r="M9" s="3">
         <v>7</v>
       </c>
-      <c r="M9" s="1" t="s">
+      <c r="N9" s="1" t="s">
         <v>64</v>
       </c>
-      <c r="N9" s="3">
+      <c r="O9" s="3">
         <v>74.5</v>
       </c>
-      <c r="O9" s="3">
+      <c r="P9" s="3">
         <v>-20.5</v>
       </c>
-      <c r="P9" s="1"/>
-      <c r="Q9" s="3">
+      <c r="Q9" s="1"/>
+      <c r="R9" s="3">
         <v>1995</v>
       </c>
-      <c r="R9" s="3">
+      <c r="S9" s="3">
         <v>2006</v>
       </c>
-      <c r="S9" s="3">
+      <c r="T9" s="3">
         <v>2004</v>
       </c>
-      <c r="T9" s="3">
+      <c r="U9" s="3">
         <v>7</v>
       </c>
-      <c r="U9" s="1"/>
-      <c r="V9" s="1" t="s">
+      <c r="V9" s="1"/>
+      <c r="W9" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="W9" s="1" t="s">
+      <c r="X9" s="1" t="s">
         <v>65</v>
       </c>
-      <c r="X9" s="1" t="s">
+      <c r="Y9" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="Y9" s="1" t="s">
+      <c r="Z9" s="1" t="s">
         <v>26</v>
-      </c>
-      <c r="Z9" s="3">
-        <v>1</v>
       </c>
       <c r="AA9" s="3">
         <v>1</v>
       </c>
-      <c r="AB9" s="1" t="s">
+      <c r="AB9" s="3">
+        <v>1</v>
+      </c>
+      <c r="AC9" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="AC9" s="1">
+      <c r="AD9" s="1">
         <v>0</v>
       </c>
-      <c r="AD9" s="1">
+      <c r="AE9" s="1">
         <v>10</v>
       </c>
-      <c r="AE9" s="1">
+      <c r="AF9" s="1">
         <v>100</v>
       </c>
-      <c r="AF9" s="1">
+      <c r="AG9" s="1">
         <v>130</v>
       </c>
-      <c r="AG9" s="1"/>
       <c r="AH9" s="1"/>
       <c r="AI9" s="1"/>
+      <c r="AJ9" s="1"/>
     </row>
-    <row r="10" spans="1:35" ht="17" thickBot="1">
+    <row r="10" spans="1:36" ht="17" thickBot="1">
       <c r="A10" s="1" t="s">
         <v>47</v>
       </c>
       <c r="B10" s="1" t="s">
         <v>66</v>
       </c>
-      <c r="C10" s="1" t="s">
+      <c r="C10" s="1"/>
+      <c r="D10" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="D10" s="1" t="s">
+      <c r="E10" s="1" t="s">
         <v>67</v>
       </c>
-      <c r="E10" s="3">
+      <c r="F10" s="3">
         <v>2003</v>
       </c>
-      <c r="F10" s="1" t="s">
+      <c r="G10" s="1" t="s">
         <v>68</v>
       </c>
-      <c r="G10" s="3">
+      <c r="H10" s="3">
         <v>73</v>
       </c>
-      <c r="H10" s="3">
+      <c r="I10" s="3">
         <v>69</v>
       </c>
-      <c r="I10" s="1" t="s">
+      <c r="J10" s="1" t="s">
         <v>52</v>
       </c>
-      <c r="J10" s="1"/>
-      <c r="K10" s="1" t="s">
+      <c r="K10" s="1"/>
+      <c r="L10" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="L10" s="3">
+      <c r="M10" s="3">
         <v>10</v>
       </c>
-      <c r="M10" s="1" t="s">
+      <c r="N10" s="1" t="s">
         <v>69</v>
       </c>
-      <c r="N10" s="3">
+      <c r="O10" s="3">
         <v>38.883000000000003</v>
       </c>
-      <c r="O10" s="3">
+      <c r="P10" s="3">
         <v>-107.033</v>
       </c>
-      <c r="P10" s="3">
+      <c r="Q10" s="3">
         <v>2920</v>
       </c>
-      <c r="Q10" s="3">
+      <c r="R10" s="3">
         <v>1995</v>
       </c>
-      <c r="R10" s="3">
+      <c r="S10" s="3">
         <v>1998</v>
       </c>
-      <c r="S10" s="3">
+      <c r="T10" s="3">
         <v>1991</v>
       </c>
-      <c r="T10" s="3">
+      <c r="U10" s="3">
         <v>7</v>
       </c>
-      <c r="U10" s="1" t="s">
+      <c r="V10" s="1" t="s">
         <v>70</v>
       </c>
-      <c r="V10" s="1" t="s">
+      <c r="W10" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="W10" s="1" t="s">
+      <c r="X10" s="1" t="s">
         <v>65</v>
       </c>
-      <c r="X10" s="1" t="s">
+      <c r="Y10" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="Y10" s="1" t="s">
+      <c r="Z10" s="1" t="s">
         <v>26</v>
-      </c>
-      <c r="Z10" s="3">
-        <v>2</v>
       </c>
       <c r="AA10" s="3">
         <v>2</v>
@@ -1670,156 +1732,162 @@
       <c r="AB10" s="3">
         <v>2</v>
       </c>
-      <c r="AC10" s="1">
+      <c r="AC10" s="3">
+        <v>2</v>
+      </c>
+      <c r="AD10" s="1">
         <v>5</v>
       </c>
-      <c r="AD10" s="1">
+      <c r="AE10" s="1">
         <v>12</v>
       </c>
-      <c r="AE10" s="1">
+      <c r="AF10" s="1">
         <v>25</v>
       </c>
-      <c r="AF10" s="1"/>
       <c r="AG10" s="1"/>
       <c r="AH10" s="1"/>
       <c r="AI10" s="1"/>
+      <c r="AJ10" s="1"/>
     </row>
-    <row r="11" spans="1:35" ht="17" thickBot="1">
-      <c r="A11" s="4" t="s">
+    <row r="11" spans="1:36" s="8" customFormat="1" ht="17" thickBot="1">
+      <c r="A11" s="5" t="s">
         <v>47</v>
       </c>
-      <c r="B11" s="1" t="s">
+      <c r="B11" s="6" t="s">
         <v>71</v>
       </c>
-      <c r="C11" s="1" t="s">
+      <c r="C11" s="6" t="s">
+        <v>106</v>
+      </c>
+      <c r="D11" s="6" t="s">
         <v>46</v>
       </c>
-      <c r="D11" s="1" t="s">
+      <c r="E11" s="6" t="s">
         <v>72</v>
       </c>
-      <c r="E11" s="3">
+      <c r="F11" s="7">
         <v>1999</v>
       </c>
-      <c r="F11" s="1" t="s">
+      <c r="G11" s="6" t="s">
         <v>73</v>
       </c>
-      <c r="G11" s="1"/>
-      <c r="H11" s="1"/>
-      <c r="I11" s="1" t="s">
+      <c r="H11" s="6"/>
+      <c r="I11" s="6"/>
+      <c r="J11" s="6" t="s">
         <v>74</v>
       </c>
-      <c r="J11" s="1"/>
-      <c r="K11" s="1" t="s">
+      <c r="K11" s="6"/>
+      <c r="L11" s="6" t="s">
         <v>22</v>
       </c>
-      <c r="L11" s="3">
+      <c r="M11" s="7">
         <v>3</v>
       </c>
-      <c r="M11" s="1" t="s">
+      <c r="N11" s="6" t="s">
         <v>32</v>
       </c>
-      <c r="N11" s="3">
+      <c r="O11" s="7">
         <v>42.54</v>
       </c>
-      <c r="O11" s="3">
+      <c r="P11" s="7">
         <v>-72.180000000000007</v>
       </c>
-      <c r="P11" s="3">
+      <c r="Q11" s="7">
         <v>365</v>
       </c>
-      <c r="Q11" s="3">
+      <c r="R11" s="7">
         <v>1993</v>
       </c>
-      <c r="R11" s="3">
+      <c r="S11" s="7">
         <v>1993</v>
       </c>
-      <c r="S11" s="3">
+      <c r="T11" s="7">
         <v>1991</v>
       </c>
-      <c r="T11" s="3">
+      <c r="U11" s="7">
         <v>20</v>
       </c>
-      <c r="U11" s="1"/>
-      <c r="V11" s="1" t="s">
+      <c r="V11" s="6"/>
+      <c r="W11" s="6" t="s">
         <v>24</v>
       </c>
-      <c r="W11" s="1" t="s">
+      <c r="X11" s="6" t="s">
         <v>65</v>
       </c>
-      <c r="X11" s="1" t="s">
+      <c r="Y11" s="6" t="s">
         <v>35</v>
       </c>
-      <c r="Y11" s="1" t="s">
+      <c r="Z11" s="6" t="s">
         <v>26</v>
       </c>
-      <c r="Z11" s="1"/>
-      <c r="AA11" s="3">
+      <c r="AA11" s="6"/>
+      <c r="AB11" s="7">
         <v>24</v>
       </c>
-      <c r="AB11" s="3">
+      <c r="AC11" s="7">
         <v>4</v>
       </c>
-      <c r="AC11" s="1">
+      <c r="AD11" s="6">
         <v>0</v>
       </c>
-      <c r="AD11" s="1">
+      <c r="AE11" s="6">
         <v>2</v>
       </c>
-      <c r="AE11" s="1">
+      <c r="AF11" s="6">
         <v>4</v>
       </c>
-      <c r="AF11" s="1"/>
-      <c r="AG11" s="1"/>
-      <c r="AH11" s="1"/>
-      <c r="AI11" s="1"/>
+      <c r="AG11" s="6"/>
+      <c r="AH11" s="6"/>
+      <c r="AI11" s="6"/>
+      <c r="AJ11" s="6"/>
     </row>
-    <row r="12" spans="1:35" ht="17" thickBot="1">
+    <row r="12" spans="1:36" ht="17" thickBot="1">
       <c r="A12" s="1" t="s">
         <v>47</v>
       </c>
       <c r="B12" s="1" t="s">
         <v>75</v>
       </c>
-      <c r="C12" s="1" t="s">
+      <c r="C12" s="1"/>
+      <c r="D12" s="1" t="s">
         <v>76</v>
       </c>
-      <c r="D12" s="1" t="s">
+      <c r="E12" s="1" t="s">
         <v>77</v>
       </c>
-      <c r="E12" s="1"/>
       <c r="F12" s="1"/>
       <c r="G12" s="1"/>
       <c r="H12" s="1"/>
-      <c r="I12" s="1" t="s">
+      <c r="I12" s="1"/>
+      <c r="J12" s="1" t="s">
         <v>78</v>
       </c>
-      <c r="J12" s="1"/>
-      <c r="K12" s="1" t="s">
+      <c r="K12" s="1"/>
+      <c r="L12" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="L12" s="1"/>
-      <c r="M12" s="1" t="s">
+      <c r="M12" s="1"/>
+      <c r="N12" s="1" t="s">
         <v>79</v>
       </c>
-      <c r="N12" s="3">
+      <c r="O12" s="3">
         <v>74.3</v>
       </c>
-      <c r="O12" s="3">
+      <c r="P12" s="3">
         <v>-21</v>
       </c>
-      <c r="P12" s="3">
+      <c r="Q12" s="3">
         <v>25</v>
       </c>
-      <c r="Q12" s="3">
+      <c r="R12" s="3">
         <v>2004</v>
       </c>
-      <c r="R12" s="3">
+      <c r="S12" s="3">
         <v>2007</v>
       </c>
-      <c r="S12" s="3">
+      <c r="T12" s="3">
         <v>1999</v>
       </c>
-      <c r="T12" s="1"/>
       <c r="U12" s="1"/>
       <c r="V12" s="1"/>
       <c r="W12" s="1"/>
@@ -1835,6 +1903,7 @@
       <c r="AG12" s="1"/>
       <c r="AH12" s="1"/>
       <c r="AI12" s="1"/>
+      <c r="AJ12" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>